<commit_message>
add the simple definition as well to show the contrast
</commit_message>
<xml_diff>
--- a/src/test/resources/examples/medium_article_example.xlsx
+++ b/src/test/resources/examples/medium_article_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antonle/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antonle/Developer/vortexa/refinery/src/test/resources/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2442FF91-848F-F842-92F0-A691F7533FEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C53481A-1DE5-504F-9B84-CD15D17E367A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4880" yWindow="2460" windowWidth="14740" windowHeight="11400" xr2:uid="{3005CCFE-4BC4-E544-828C-AA7AB6E70C7F}"/>
+    <workbookView xWindow="4880" yWindow="2460" windowWidth="14740" windowHeight="11400" activeTab="1" xr2:uid="{3005CCFE-4BC4-E544-828C-AA7AB6E70C7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Awesome port" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="21">
   <si>
     <t>Report date</t>
   </si>
@@ -62,27 +62,6 @@
     <t>Crude oil</t>
   </si>
   <si>
-    <t>Lorem</t>
-  </si>
-  <si>
-    <t>Ipsum</t>
-  </si>
-  <si>
-    <t>Dolor</t>
-  </si>
-  <si>
-    <t>Sit</t>
-  </si>
-  <si>
-    <t>Amet</t>
-  </si>
-  <si>
-    <t>Consectetur</t>
-  </si>
-  <si>
-    <t>Adipiscing</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -101,17 +80,32 @@
     <t>Awesome port</t>
   </si>
   <si>
-    <t xml:space="preserve">Lorem </t>
-  </si>
-  <si>
-    <t>Crude Oil</t>
+    <t>Titanic</t>
+  </si>
+  <si>
+    <t>Black Pearl</t>
+  </si>
+  <si>
+    <t>Ever Given</t>
+  </si>
+  <si>
+    <t>Cutty Sark</t>
+  </si>
+  <si>
+    <t>USS Enterprise</t>
+  </si>
+  <si>
+    <t>Flying Dutchman</t>
+  </si>
+  <si>
+    <t>Interceptor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -131,13 +125,6 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -190,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -201,13 +188,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -526,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67EA4453-29C1-9748-AB3E-ABF625DA1988}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -559,21 +545,21 @@
         <v>3</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="11">
+        <v>14</v>
+      </c>
+      <c r="B6" s="10">
         <v>44653</v>
       </c>
       <c r="C6" s="9">
@@ -582,9 +568,9 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="11">
+        <v>16</v>
+      </c>
+      <c r="B7" s="10">
         <v>44654</v>
       </c>
       <c r="C7" s="9">
@@ -592,17 +578,17 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="11">
+        <v>17</v>
+      </c>
+      <c r="B9" s="10">
         <v>44654</v>
       </c>
       <c r="C9" s="9">
@@ -611,9 +597,9 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="11">
+        <v>18</v>
+      </c>
+      <c r="B10" s="10">
         <v>44657</v>
       </c>
       <c r="C10" s="9">
@@ -635,21 +621,21 @@
         <v>5</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="11">
+        <v>15</v>
+      </c>
+      <c r="B15" s="10">
         <v>44650</v>
       </c>
       <c r="C15" s="9">
@@ -658,9 +644,9 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="11">
+        <v>19</v>
+      </c>
+      <c r="B16" s="10">
         <v>44651</v>
       </c>
       <c r="C16" s="9">
@@ -668,17 +654,17 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="11">
+        <v>20</v>
+      </c>
+      <c r="B18" s="10">
         <v>44652</v>
       </c>
       <c r="C18" s="9">
@@ -700,13 +686,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD22092E-EC73-A04F-BB63-F0B67FCF0CC4}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="7" max="7" width="15.33203125" customWidth="1"/>
   </cols>
@@ -716,22 +703,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -742,19 +729,19 @@
         <v>1</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="13">
+        <v>14</v>
+      </c>
+      <c r="D2" s="11">
         <v>44653</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="F2">
         <v>10000</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -765,19 +752,19 @@
         <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="13">
+        <v>16</v>
+      </c>
+      <c r="D3" s="11">
         <v>44654</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="F3">
         <v>20000</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -788,9 +775,9 @@
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="13">
+        <v>17</v>
+      </c>
+      <c r="D4" s="11">
         <v>44654</v>
       </c>
       <c r="E4" t="s">
@@ -800,7 +787,7 @@
         <v>40000</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -811,9 +798,9 @@
         <v>1</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="13">
+        <v>18</v>
+      </c>
+      <c r="D5" s="11">
         <v>44657</v>
       </c>
       <c r="E5" t="s">
@@ -823,7 +810,7 @@
         <v>80000</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -834,19 +821,19 @@
         <v>2</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="13">
+        <v>15</v>
+      </c>
+      <c r="D6" s="11">
         <v>44650</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>22</v>
+      <c r="E6" t="s">
+        <v>7</v>
       </c>
       <c r="F6">
         <v>40000</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -857,19 +844,19 @@
         <v>2</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="13">
+        <v>19</v>
+      </c>
+      <c r="D7" s="11">
         <v>44651</v>
       </c>
-      <c r="E7" s="12" t="s">
-        <v>22</v>
+      <c r="E7" t="s">
+        <v>7</v>
       </c>
       <c r="F7">
         <v>20000</v>
       </c>
       <c r="G7" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -880,9 +867,9 @@
         <v>2</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="13">
+        <v>20</v>
+      </c>
+      <c r="D8" s="11">
         <v>44652</v>
       </c>
       <c r="E8" t="s">
@@ -892,7 +879,7 @@
         <v>10000</v>
       </c>
       <c r="G8" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -912,5 +899,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>